<commit_message>
EPBDS-7379 Add support autocast types to Range types. Add tests.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="673">
   <si>
     <t>Step</t>
   </si>
@@ -1387,9 +1387,6 @@
     <t>Spreadsheet SpreadsheetResult ExplicitPrimitivesCasts()</t>
   </si>
   <si>
-    <t>= (Character)((Character) 0)</t>
-  </si>
-  <si>
     <t>= (Character)((char) 0)</t>
   </si>
   <si>
@@ -1408,9 +1405,6 @@
     <t>= (Character)((double) 0)</t>
   </si>
   <si>
-    <t>= (Short)((Short) 0)</t>
-  </si>
-  <si>
     <t>= (Short)((char) 0)</t>
   </si>
   <si>
@@ -1429,9 +1423,6 @@
     <t>= (Short)((double) 0)</t>
   </si>
   <si>
-    <t>= (Integer)((Integer) 0)</t>
-  </si>
-  <si>
     <t>= (Integer)((char) 0)</t>
   </si>
   <si>
@@ -1450,9 +1441,6 @@
     <t>= (Integer)((double) 0)</t>
   </si>
   <si>
-    <t>= (Long)((Long) 0)</t>
-  </si>
-  <si>
     <t>= (Long)((char) 0)</t>
   </si>
   <si>
@@ -1471,9 +1459,6 @@
     <t>= (Long)((double) 0)</t>
   </si>
   <si>
-    <t>= (Float)((Float) 0)</t>
-  </si>
-  <si>
     <t>= (Float)((char) 0)</t>
   </si>
   <si>
@@ -1492,9 +1477,6 @@
     <t>= (Float)((double) 0)</t>
   </si>
   <si>
-    <t>= (Double)((Double) 0)</t>
-  </si>
-  <si>
     <t>= (Double)((char) 0)</t>
   </si>
   <si>
@@ -1513,9 +1495,6 @@
     <t>= (Double)((double) 0)</t>
   </si>
   <si>
-    <t>= (BigInteger)((BigInteger) 0)</t>
-  </si>
-  <si>
     <t>= (BigInteger)((char) 0)</t>
   </si>
   <si>
@@ -1534,9 +1513,6 @@
     <t>= (BigInteger)((double) 0)</t>
   </si>
   <si>
-    <t>= (BigDecimal)((BigDecimal) 0)</t>
-  </si>
-  <si>
     <t>= (BigDecimal)((char) 0)</t>
   </si>
   <si>
@@ -1555,9 +1531,6 @@
     <t>= (BigDecimal)((double) 0)</t>
   </si>
   <si>
-    <t>= (ByteValue)((ByteValue) 0)</t>
-  </si>
-  <si>
     <t>= (ByteValue)((char) 0)</t>
   </si>
   <si>
@@ -1576,9 +1549,6 @@
     <t>= (ByteValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (ShortValue)((ShortValue) 0)</t>
-  </si>
-  <si>
     <t>= (ShortValue)((char) 0)</t>
   </si>
   <si>
@@ -1597,9 +1567,6 @@
     <t>= (ShortValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (IntValue)((IntValue) 0)</t>
-  </si>
-  <si>
     <t>= (IntValue)((char) 0)</t>
   </si>
   <si>
@@ -1618,9 +1585,6 @@
     <t>= (IntValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (LongValue)((LongValue) 0)</t>
-  </si>
-  <si>
     <t>= (LongValue)((char) 0)</t>
   </si>
   <si>
@@ -1639,9 +1603,6 @@
     <t>= (LongValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (FloatValue)((FloatValue) 0)</t>
-  </si>
-  <si>
     <t>= (FloatValue)((char) 0)</t>
   </si>
   <si>
@@ -1660,9 +1621,6 @@
     <t>= (FloatValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (DoubleValue)((DoubleValue) 0)</t>
-  </si>
-  <si>
     <t>= (DoubleValue)((char) 0)</t>
   </si>
   <si>
@@ -1681,9 +1639,6 @@
     <t>= (DoubleValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (BigIntegerValue)((BigIntegerValue) 0)</t>
-  </si>
-  <si>
     <t>= (BigIntegerValue)((char) 0)</t>
   </si>
   <si>
@@ -1702,9 +1657,6 @@
     <t>= (BigIntegerValue)((double) 0)</t>
   </si>
   <si>
-    <t>= (BigDecimalValue)((BigDecimalValue) 0)</t>
-  </si>
-  <si>
     <t>= (BigDecimalValue)((char) 0)</t>
   </si>
   <si>
@@ -1880,13 +1832,223 @@
   </si>
   <si>
     <t>= Double.valueOf((double)((double) 0))</t>
+  </si>
+  <si>
+    <t>IntRange</t>
+  </si>
+  <si>
+    <t>= new IntRange(0);</t>
+  </si>
+  <si>
+    <t>DoubleRange</t>
+  </si>
+  <si>
+    <t>= new DoubleRange(0);</t>
+  </si>
+  <si>
+    <t>IntRange : IntRange</t>
+  </si>
+  <si>
+    <t>DoubleRange : DoubleRange</t>
+  </si>
+  <si>
+    <t>CharRange</t>
+  </si>
+  <si>
+    <t>= new CharRange('a');</t>
+  </si>
+  <si>
+    <t>CharRange : CharRange</t>
+  </si>
+  <si>
+    <t>=(char) 0</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$Byte</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$Short</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$Integer</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$Long</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$Float</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$Double</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$BigInteger</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$BigDecimal</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$ByteValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$ShortValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$IntValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$LongValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$FloatValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$DoubleValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$BigIntegerValue</t>
+  </si>
+  <si>
+    <t>= (IntRange)$Types.$Value$IntRange</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$Byte</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$Short</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$Integer</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$Long</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$Float</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$Double</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$BigInteger</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$BigDecimal</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$ByteValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$ShortValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$IntValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$LongValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$FloatValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$DoubleValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$BigIntegerValue</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)$Types.$Value$DoubleRange</t>
+  </si>
+  <si>
+    <t>= (CharRange)$Types.$Value$Character</t>
+  </si>
+  <si>
+    <t>= (CharRange)((char) 0)</t>
+  </si>
+  <si>
+    <t>= (Character)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (Short)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (Integer)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (Long)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (BigInteger)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (BigDecimal)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (ByteValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (ShortValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (IntValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (LongValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (FloatValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (BigIntegerValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (BigDecimalValue)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (IntRange)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)((byte) 0)</t>
+  </si>
+  <si>
+    <t>= (IntRange)((short) 0)</t>
+  </si>
+  <si>
+    <t>= (IntRange)((int) 0)</t>
+  </si>
+  <si>
+    <t>= (IntRange)((long) 0)</t>
+  </si>
+  <si>
+    <t>= (IntRange)((float) 0)</t>
+  </si>
+  <si>
+    <t>= (IntRange)((double) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)((short) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)((int) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)((long) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)((float) 0)</t>
+  </si>
+  <si>
+    <t>= (DoubleRange)((double) 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1922,7 +2084,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1950,6 +2112,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6DB66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2058,34 +2226,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2427,27 +2604,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:D25"/>
+  <dimension ref="C5:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="37.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="65" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4">
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:4">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="15.75" thickBot="1">
+    <row r="7" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2463,7 +2640,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="18" customHeight="1" thickBot="1">
+    <row r="8" spans="3:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
@@ -2471,7 +2648,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="3:4" ht="14.25" customHeight="1" thickBot="1">
+    <row r="9" spans="3:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
@@ -2479,7 +2656,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="3:4" ht="15.75" customHeight="1" thickBot="1">
+    <row r="10" spans="3:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
@@ -2487,7 +2664,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="11" spans="3:4" ht="15.75" thickBot="1">
+    <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2495,7 +2672,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="3:4" ht="15.75" thickBot="1">
+    <row r="12" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
@@ -2503,7 +2680,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="3:4" ht="15.75" thickBot="1">
+    <row r="13" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2511,7 +2688,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="14" spans="3:4" ht="15.75" thickBot="1">
+    <row r="14" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
@@ -2519,7 +2696,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="15" spans="3:4" ht="15.75" thickBot="1">
+    <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
@@ -2527,7 +2704,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="16" spans="3:4" ht="15.75" thickBot="1">
+    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
@@ -2535,7 +2712,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="15.75" thickBot="1">
+    <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
@@ -2543,7 +2720,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="15.75" thickBot="1">
+    <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
@@ -2551,7 +2728,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="15.75" thickBot="1">
+    <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
@@ -2559,7 +2736,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="15.75" thickBot="1">
+    <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
@@ -2567,7 +2744,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="21" spans="3:4" ht="15.75" thickBot="1">
+    <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
@@ -2575,7 +2752,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="15.75" thickBot="1">
+    <row r="22" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
@@ -2583,7 +2760,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="23" spans="3:4" ht="15.75" thickBot="1">
+    <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
@@ -2591,7 +2768,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="24" spans="3:4">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>384</v>
       </c>
@@ -2599,12 +2776,36 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>387</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>388</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -2617,15 +2818,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:V59"/>
+  <dimension ref="C4:V62"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:J59"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1" collapsed="1"/>
@@ -2642,31 +2843,31 @@
     <col min="20" max="22" width="24.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22">
-      <c r="C4" s="11" t="s">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-    </row>
-    <row r="5" spans="3:22">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2728,7 +2929,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="6" spans="3:22" ht="15.75" thickBot="1">
+    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -2790,7 +2991,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="3:22" ht="15.75" thickBot="1">
+    <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -2816,7 +3017,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="3:22" ht="15.75" thickBot="1">
+    <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
@@ -2842,7 +3043,7 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" spans="3:22" ht="18" customHeight="1" thickBot="1">
+    <row r="9" spans="3:22" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
@@ -2870,7 +3071,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" spans="3:22" ht="15.75" thickBot="1">
+    <row r="10" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
@@ -2902,7 +3103,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="3:22" ht="15.75" thickBot="1">
+    <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
@@ -2936,7 +3137,7 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
-    <row r="12" spans="3:22" ht="15.75" thickBot="1">
+    <row r="12" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
@@ -2972,7 +3173,7 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="3:22" ht="15.75" thickBot="1">
+    <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
@@ -3010,7 +3211,7 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
-    <row r="14" spans="3:22" ht="15.75" thickBot="1">
+    <row r="14" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3046,7 +3247,7 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
     </row>
-    <row r="15" spans="3:22" ht="39" thickBot="1">
+    <row r="15" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
@@ -3088,7 +3289,7 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
     </row>
-    <row r="16" spans="3:22" ht="15.75" thickBot="1">
+    <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
@@ -3116,7 +3317,7 @@
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
     </row>
-    <row r="17" spans="3:22" ht="15.75" thickBot="1">
+    <row r="17" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
@@ -3148,7 +3349,7 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
     </row>
-    <row r="18" spans="3:22" ht="39" thickBot="1">
+    <row r="18" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
@@ -3186,7 +3387,7 @@
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
     </row>
-    <row r="19" spans="3:22" ht="39" thickBot="1">
+    <row r="19" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
@@ -3228,7 +3429,7 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
     </row>
-    <row r="20" spans="3:22" ht="39" thickBot="1">
+    <row r="20" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
@@ -3274,7 +3475,7 @@
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
     </row>
-    <row r="21" spans="3:22" ht="39" thickBot="1">
+    <row r="21" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
@@ -3324,7 +3525,7 @@
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
     </row>
-    <row r="22" spans="3:22" ht="39" thickBot="1">
+    <row r="22" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3370,7 +3571,7 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
     </row>
-    <row r="23" spans="3:22" ht="39" thickBot="1">
+    <row r="23" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
@@ -3428,7 +3629,7 @@
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
     </row>
-    <row r="24" spans="3:22" ht="39" thickBot="1">
+    <row r="24" spans="3:22" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>390</v>
       </c>
@@ -3456,7 +3657,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="3:22" ht="15.75" thickBot="1">
+    <row r="25" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>402</v>
       </c>
@@ -3482,19 +3683,111 @@
         <v>404</v>
       </c>
     </row>
-    <row r="34" spans="3:10">
-      <c r="C34" s="11" t="s">
+    <row r="26" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+    </row>
+    <row r="27" spans="3:22" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+    </row>
+    <row r="28" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-    </row>
-    <row r="35" spans="3:10">
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>0</v>
       </c>
@@ -3520,7 +3813,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="15.75" thickBot="1">
+    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
         <v>22</v>
       </c>
@@ -3534,7 +3827,7 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="3:10" ht="15.75" thickBot="1">
+    <row r="37" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
         <v>27</v>
       </c>
@@ -3548,7 +3841,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="3:10" ht="15.75" thickBot="1">
+    <row r="38" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
         <v>26</v>
       </c>
@@ -3564,7 +3857,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="3:10" ht="15.75" thickBot="1">
+    <row r="39" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
         <v>28</v>
       </c>
@@ -3584,7 +3877,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="3:10" ht="15.75" thickBot="1">
+    <row r="40" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
         <v>29</v>
       </c>
@@ -3606,7 +3899,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="3:10" ht="15.75" thickBot="1">
+    <row r="41" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>30</v>
       </c>
@@ -3630,7 +3923,7 @@
       </c>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="3:10" ht="15.75" thickBot="1">
+    <row r="42" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>31</v>
       </c>
@@ -3656,7 +3949,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="43" spans="3:10" ht="15.75" thickBot="1">
+    <row r="43" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
         <v>32</v>
       </c>
@@ -3678,7 +3971,7 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="3:10" ht="26.25" thickBot="1">
+    <row r="44" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>33</v>
       </c>
@@ -3704,7 +3997,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="15.75" thickBot="1">
+    <row r="45" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>34</v>
       </c>
@@ -3718,7 +4011,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="3:10" ht="15.75" thickBot="1">
+    <row r="46" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>35</v>
       </c>
@@ -3734,7 +4027,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="3:10" ht="15.75" thickBot="1">
+    <row r="47" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>36</v>
       </c>
@@ -3754,7 +4047,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="3:10" ht="15.75" thickBot="1">
+    <row r="48" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
         <v>37</v>
       </c>
@@ -3776,7 +4069,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="3:10" ht="15.75" thickBot="1">
+    <row r="49" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
         <v>38</v>
       </c>
@@ -3800,7 +4093,7 @@
       </c>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="3:10" ht="26.25" thickBot="1">
+    <row r="50" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
         <v>39</v>
       </c>
@@ -3826,7 +4119,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="26.25" thickBot="1">
+    <row r="51" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
         <v>40</v>
       </c>
@@ -3848,7 +4141,7 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="3:10" ht="26.25" thickBot="1">
+    <row r="52" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
         <v>41</v>
       </c>
@@ -3874,139 +4167,195 @@
         <v>412</v>
       </c>
     </row>
-    <row r="53" spans="3:10" ht="15.75" thickBot="1">
+    <row r="53" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
-        <v>413</v>
+        <v>607</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="F53" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>409</v>
+      </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="3:10" ht="15.75" thickBot="1">
+    <row r="54" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-    </row>
-    <row r="55" spans="3:10" ht="15.75" thickBot="1">
+        <v>608</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4" t="s">
-        <v>435</v>
-      </c>
+        <v>611</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="3:10" ht="15.75" thickBot="1">
+    <row r="56" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>436</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="3:10" ht="15.75" thickBot="1">
+    <row r="57" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>421</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>440</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="3:10" ht="15.75" thickBot="1">
+    <row r="58" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="G61" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I61" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="J58" s="4"/>
-    </row>
-    <row r="59" spans="3:10" ht="26.25" thickBot="1">
-      <c r="C59" s="3" t="s">
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F62" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="G62" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="I62" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>445</v>
       </c>
     </row>
@@ -4021,39 +4370,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:V55"/>
+  <dimension ref="C4:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55:J55"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:22">
-      <c r="C4" s="12" t="s">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-    </row>
-    <row r="5" spans="3:22">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -4115,7 +4485,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="6" spans="3:22" ht="26.25" thickBot="1">
+    <row r="6" spans="3:22" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -4177,7 +4547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="3:22" ht="77.25" thickBot="1">
+    <row r="7" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -4235,7 +4605,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="3:22" ht="77.25" thickBot="1">
+    <row r="8" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
@@ -4293,7 +4663,7 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" spans="3:22" ht="77.25" thickBot="1">
+    <row r="9" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
@@ -4351,7 +4721,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" spans="3:22" ht="77.25" thickBot="1">
+    <row r="10" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
@@ -4409,7 +4779,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="3:22" ht="77.25" thickBot="1">
+    <row r="11" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
@@ -4467,7 +4837,7 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
-    <row r="12" spans="3:22" ht="77.25" thickBot="1">
+    <row r="12" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
@@ -4525,7 +4895,7 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="3:22" ht="77.25" thickBot="1">
+    <row r="13" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
@@ -4583,7 +4953,7 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
-    <row r="14" spans="3:22" ht="77.25" thickBot="1">
+    <row r="14" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
@@ -4641,7 +5011,7 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
     </row>
-    <row r="15" spans="3:22" ht="77.25" thickBot="1">
+    <row r="15" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
@@ -4699,7 +5069,7 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
     </row>
-    <row r="16" spans="3:22" ht="77.25" thickBot="1">
+    <row r="16" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
@@ -4757,7 +5127,7 @@
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
     </row>
-    <row r="17" spans="3:22" ht="77.25" thickBot="1">
+    <row r="17" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
@@ -4815,7 +5185,7 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
     </row>
-    <row r="18" spans="3:22" ht="77.25" thickBot="1">
+    <row r="18" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
@@ -4873,7 +5243,7 @@
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
     </row>
-    <row r="19" spans="3:22" ht="77.25" thickBot="1">
+    <row r="19" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
@@ -4931,7 +5301,7 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
     </row>
-    <row r="20" spans="3:22" ht="77.25" thickBot="1">
+    <row r="20" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
@@ -4989,7 +5359,7 @@
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
     </row>
-    <row r="21" spans="3:22" ht="77.25" thickBot="1">
+    <row r="21" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
@@ -5047,7 +5417,7 @@
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
     </row>
-    <row r="22" spans="3:22" ht="90" thickBot="1">
+    <row r="22" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
@@ -5105,7 +5475,7 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
     </row>
-    <row r="23" spans="3:22" ht="90" thickBot="1">
+    <row r="23" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
@@ -5163,7 +5533,7 @@
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
     </row>
-    <row r="24" spans="3:22" ht="77.25" thickBot="1">
+    <row r="24" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>390</v>
       </c>
@@ -5191,7 +5561,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="25" spans="3:22" ht="64.5" thickBot="1">
+    <row r="25" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>391</v>
       </c>
@@ -5219,672 +5589,872 @@
         <v>397</v>
       </c>
     </row>
-    <row r="30" spans="3:22">
-      <c r="C30" s="11" t="s">
+    <row r="26" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+    </row>
+    <row r="27" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+    </row>
+    <row r="28" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+    </row>
+    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C32" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="3:22">
-      <c r="C31" s="6" t="s">
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I33" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="32" spans="3:22" ht="39" thickBot="1">
-      <c r="C32" s="3" t="s">
+    <row r="34" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C33" s="3" t="s">
+    <row r="35" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="J33" s="4" t="s">
+    </row>
+    <row r="36" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="34" spans="3:10" ht="39" thickBot="1">
-      <c r="C34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="I34" s="4" t="s">
+    </row>
+    <row r="37" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="35" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="J37" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="H35" s="4" t="s">
+    </row>
+    <row r="38" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="36" spans="3:10" ht="39" thickBot="1">
-      <c r="C36" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="J38" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="G36" s="4" t="s">
+    </row>
+    <row r="39" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="37" spans="3:10" ht="39" thickBot="1">
-      <c r="C37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="I39" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="J39" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="F37" s="4" t="s">
+    </row>
+    <row r="40" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="I40" s="4" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="38" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="J40" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="E38" s="4" t="s">
+    </row>
+    <row r="41" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H41" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="39" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C39" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="4" t="s">
+    <row r="42" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="J39" s="4" t="s">
+    </row>
+    <row r="43" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="40" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C40" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="I43" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="I40" s="4" t="s">
+    </row>
+    <row r="44" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="41" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C41" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="I44" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="J44" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="H41" s="4" t="s">
+    </row>
+    <row r="45" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="42" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C42" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="G42" s="4" t="s">
+    </row>
+    <row r="46" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="43" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C43" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="J46" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="F43" s="4" t="s">
+    </row>
+    <row r="47" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="44" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="E44" s="4" t="s">
+    </row>
+    <row r="48" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H48" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I48" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J48" s="4" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="51.75" thickBot="1">
-      <c r="C45" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="4" t="s">
+    <row r="49" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I49" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="J49" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="J45" s="4" t="s">
+    </row>
+    <row r="50" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="46" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C46" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="I50" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="J50" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C47" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>553</v>
-      </c>
-      <c r="F47" s="4" t="s">
+    </row>
+    <row r="51" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+    </row>
+    <row r="54" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="G54" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="H54" s="4" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="48" spans="3:10" ht="77.25" thickBot="1">
-      <c r="C48" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="F48" s="4" t="s">
+    </row>
+    <row r="55" spans="3:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="F55" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="G55" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="49" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C49" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="I55" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="G56" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="H56" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="J56" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I49" s="4" t="s">
+    </row>
+    <row r="57" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="50" spans="3:10" ht="77.25" thickBot="1">
-      <c r="C50" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="F58" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="G58" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="H58" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="I58" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="J58" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="I50" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C51" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>586</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>587</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>588</v>
-      </c>
-      <c r="I51" s="4" t="s">
+    </row>
+    <row r="59" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="J51" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="52" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C52" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="F59" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="G60" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="H60" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="I60" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="J60" s="4" t="s">
         <v>602</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="53" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C53" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>596</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="54" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C54" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>608</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10" ht="64.5" thickBot="1">
-      <c r="C55" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>612</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>618</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C4:V4"/>
-    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C32:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5894,88 +6464,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B8:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>567</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-7435 ArrayCast throws ArrayIndexOutOfBoundException
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FA09E67B-BE1B-44C9-9D30-C97307834995}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="11" r:id="rId1"/>
     <sheet name="ImplicitCasts" sheetId="12" r:id="rId2"/>
     <sheet name="ExplicitCasts" sheetId="13" r:id="rId3"/>
     <sheet name="Tests" sheetId="14" r:id="rId4"/>
+    <sheet name="ArrayCast" sheetId="15" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_st1">#REF!</definedName>
@@ -22,8 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{78E0298A-F43E-40A0-B7DB-AD9D9390A5B0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>access to the cell value of Spreadsheet Table</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="686">
   <si>
     <t>Step</t>
   </si>
@@ -2042,13 +2068,52 @@
   </si>
   <si>
     <t>= (DoubleRange)((double) 0)</t>
+  </si>
+  <si>
+    <t>A : Object</t>
+  </si>
+  <si>
+    <t>= new Integer[] {1,2,3};</t>
+  </si>
+  <si>
+    <t>B : Object</t>
+  </si>
+  <si>
+    <t>= new Integer[] {3,4,5};</t>
+  </si>
+  <si>
+    <t>C : Object</t>
+  </si>
+  <si>
+    <t>= new Object[] {$A, $B}</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>= (Integer[][]) $C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>= $D[1][1]</t>
+  </si>
+  <si>
+    <t>_res_.$Value$E</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  arrayCast()</t>
+  </si>
+  <si>
+    <t>Test arrayCast arrayCastTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2080,6 +2145,13 @@
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -2122,7 +2194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2221,12 +2293,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2265,9 +2391,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Accent1 10" xfId="1"/>
+    <cellStyle name="20% - Accent1 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2603,7 +2747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2817,7 +2961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C4:V62"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
@@ -4369,11 +4513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C4:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6207,7 +6351,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
         <v>607</v>
       </c>
@@ -6461,7 +6605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B8:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6469,6 +6613,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -6553,4 +6700,102 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1544BA-DE05-49B2-97B9-067BC3BBDAFA}">
+  <dimension ref="B5:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>684</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>673</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>675</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>677</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>679</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="27" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="22" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="23">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-8287 Move trivial tests to functionality
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FA09E67B-BE1B-44C9-9D30-C97307834995}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="11" r:id="rId1"/>
@@ -13,6 +12,7 @@
     <sheet name="ExplicitCasts" sheetId="13" r:id="rId3"/>
     <sheet name="Tests" sheetId="14" r:id="rId4"/>
     <sheet name="ArrayCast" sheetId="15" r:id="rId5"/>
+    <sheet name="AliasCast" sheetId="16" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_st1">#REF!</definedName>
@@ -25,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{78E0298A-F43E-40A0-B7DB-AD9D9390A5B0}">
+    <comment ref="C7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="710">
   <si>
     <t>Step</t>
   </si>
@@ -2107,12 +2107,84 @@
   </si>
   <si>
     <t>Test arrayCast arrayCastTest</t>
+  </si>
+  <si>
+    <t>Datatype MyAlias &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>= new String[] {"One", "Three"}</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>One, Three</t>
+  </si>
+  <si>
+    <t>Test aliasCase1</t>
+  </si>
+  <si>
+    <t>Spreadsheet MyAlias[] aliasCase1()</t>
+  </si>
+  <si>
+    <t>Spreadsheet MyAlias[] aliasCase2()</t>
+  </si>
+  <si>
+    <t>Test aliasCase2</t>
+  </si>
+  <si>
+    <t>= new String[] {"One", "Two"}</t>
+  </si>
+  <si>
+    <t>One, Two</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>= $val</t>
+  </si>
+  <si>
+    <t>Spreadsheet MyAlias[][] aliasCase3()</t>
+  </si>
+  <si>
+    <t>= new String[] {"Two", "One", "Three"}</t>
+  </si>
+  <si>
+    <t>= $val[split by substring(0,1)]</t>
+  </si>
+  <si>
+    <t>_res_[0]</t>
+  </si>
+  <si>
+    <t>_res_[1]</t>
+  </si>
+  <si>
+    <t>Two, Three</t>
+  </si>
+  <si>
+    <t>Test aliasCase3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2194,7 +2266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2347,12 +2419,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2385,15 +2483,6 @@
     <xf numFmtId="3" fontId="2" fillId="6" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2409,10 +2498,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Accent1 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent1 10" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2428,9 +2537,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2468,9 +2577,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2503,26 +2612,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2555,26 +2647,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2747,7 +2822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2761,10 +2836,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2961,7 +3036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:V62"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
@@ -2988,28 +3063,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
@@ -3920,16 +3995,16 @@
       <c r="V28" s="4"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="21" t="s">
         <v>405</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
@@ -4513,11 +4588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:V60"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,28 +4619,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
@@ -5872,16 +5947,16 @@
       <c r="V28" s="4"/>
     </row>
     <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="21" t="s">
         <v>453</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="6" t="s">
@@ -6605,7 +6680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B8:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6703,10 +6778,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1544BA-DE05-49B2-97B9-067BC3BBDAFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -6717,77 +6792,77 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="23" t="s">
         <v>684</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
         <v>673</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>675</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="17" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
         <v>677</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="17" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>679</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="17" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="27" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
         <v>681</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="17" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="19" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="19" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23">
+      <c r="B19" s="20">
         <v>4</v>
       </c>
     </row>
@@ -6798,4 +6873,173 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
+        <v>696</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="E11" s="27" t="s">
+        <v>697</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="H11" s="27" t="s">
+        <v>703</v>
+      </c>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>690</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>690</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>691</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>692</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="24" t="s">
+        <v>691</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>702</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>691</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>695</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>698</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>709</v>
+      </c>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>693</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>693</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>706</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>694</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>700</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>708</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>687</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H17:I17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-8290 Fix casting to a multidimension array of a Alias datatype
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="717">
   <si>
     <t>Step</t>
   </si>
@@ -2163,12 +2163,6 @@
     <t>Spreadsheet MyAlias[][] aliasCase3()</t>
   </si>
   <si>
-    <t>= new String[] {"Two", "One", "Three"}</t>
-  </si>
-  <si>
-    <t>= $val[split by substring(0,1)]</t>
-  </si>
-  <si>
     <t>_res_[0]</t>
   </si>
   <si>
@@ -2179,6 +2173,33 @@
   </si>
   <si>
     <t>Test aliasCase3</t>
+  </si>
+  <si>
+    <t>val2</t>
+  </si>
+  <si>
+    <t>= $val[(x) split by x.substring(0,1)]</t>
+  </si>
+  <si>
+    <t>= (MyAlias[][]) $val2</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>= new String[] {"Two", "One", "Other", "Three"}</t>
+  </si>
+  <si>
+    <t>One, Other</t>
+  </si>
+  <si>
+    <t>Spreadsheet MyAlias[] aliasCase4()</t>
+  </si>
+  <si>
+    <t>Test aliasCase4</t>
+  </si>
+  <si>
+    <t>= new MyAlias[] {"One", "Other"}</t>
   </si>
 </sst>
 </file>
@@ -2450,7 +2471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2498,6 +2519,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2507,15 +2532,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2836,10 +2859,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3063,28 +3086,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
@@ -3995,16 +4018,16 @@
       <c r="V28" s="4"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="25" t="s">
         <v>405</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
@@ -4619,28 +4642,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
@@ -5947,16 +5970,16 @@
       <c r="V28" s="4"/>
     </row>
     <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="25" t="s">
         <v>453</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="6" t="s">
@@ -6792,10 +6815,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="27" t="s">
         <v>684</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
@@ -6877,10 +6900,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:I20"/>
+  <dimension ref="B5:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6890,155 +6913,213 @@
     <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="28" t="s">
         <v>696</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="29"/>
+      <c r="E11" s="28" t="s">
         <v>697</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="H11" s="27" t="s">
+      <c r="F11" s="29"/>
+      <c r="H11" s="30" t="s">
         <v>703</v>
       </c>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="I11" s="30"/>
+      <c r="K11" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="L11" s="29"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="21" t="s">
         <v>690</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="21" t="s">
         <v>690</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="21" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="K12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>691</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>692</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="21" t="s">
         <v>701</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="22" t="s">
         <v>699</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="21" t="s">
         <v>701</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="22" t="s">
+        <v>712</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>701</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="21" t="s">
+        <v>691</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>702</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>708</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>709</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>691</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="21" t="s">
+        <v>691</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>695</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>698</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>707</v>
+      </c>
+      <c r="I19" s="30"/>
+      <c r="K19" s="21" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>693</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>693</v>
+      </c>
+      <c r="H20" s="21" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="24" t="s">
-        <v>691</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>702</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>691</v>
-      </c>
-      <c r="I14" s="25" t="s">
+      <c r="I20" s="21" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
-        <v>695</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>698</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>709</v>
-      </c>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+      <c r="K20" s="21" t="s">
         <v>693</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>693</v>
-      </c>
-      <c r="H18" s="24" t="s">
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="I21" s="21"/>
+      <c r="K21" s="21" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>694</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>700</v>
+      </c>
+      <c r="H22" s="21" t="s">
         <v>706</v>
       </c>
-      <c r="I18" s="24" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
-        <v>694</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>700</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>708</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>687</v>
+      <c r="I22" s="21" t="s">
+        <v>713</v>
+      </c>
+      <c r="K22" s="21" t="s">
+        <v>713</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="K11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-8291 User recursive algoritm for casting multidimensional arrays
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="11" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="747">
   <si>
     <t>Step</t>
   </si>
@@ -2070,45 +2070,18 @@
     <t>= (DoubleRange)((double) 0)</t>
   </si>
   <si>
-    <t>A : Object</t>
-  </si>
-  <si>
     <t>= new Integer[] {1,2,3};</t>
   </si>
   <si>
-    <t>B : Object</t>
-  </si>
-  <si>
-    <t>= new Integer[] {3,4,5};</t>
-  </si>
-  <si>
-    <t>C : Object</t>
-  </si>
-  <si>
-    <t>= new Object[] {$A, $B}</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>= (Integer[][]) $C</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>= $D[1][1]</t>
-  </si>
-  <si>
-    <t>_res_.$Value$E</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult  arrayCast()</t>
   </si>
   <si>
-    <t>Test arrayCast arrayCastTest</t>
-  </si>
-  <si>
     <t>Datatype MyAlias &lt;String&gt;</t>
   </si>
   <si>
@@ -2187,19 +2160,136 @@
     <t>Other</t>
   </si>
   <si>
-    <t>= new String[] {"Two", "One", "Other", "Three"}</t>
-  </si>
-  <si>
     <t>One, Other</t>
   </si>
   <si>
+    <t>= new String[] {"Two", "One", "Three"}</t>
+  </si>
+  <si>
+    <t>= new Integer[] {4,5};</t>
+  </si>
+  <si>
+    <t>= new Integer[] {};</t>
+  </si>
+  <si>
+    <t>= new Integer[] {6};</t>
+  </si>
+  <si>
+    <t>= new Object[] {$A, $B, $C, $D}</t>
+  </si>
+  <si>
+    <t>= new Object[] {$D, $C, $B, $A}</t>
+  </si>
+  <si>
+    <t>= new Object[] {$D}</t>
+  </si>
+  <si>
+    <t>= new Object[] {$B, $B}</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>= (Integer[][]) $obj</t>
+  </si>
+  <si>
+    <t>obj</t>
+  </si>
+  <si>
+    <t>= new Integer[][] {$obj}</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>= sum($2D)</t>
+  </si>
+  <si>
+    <t>_res_.$sum$A</t>
+  </si>
+  <si>
+    <t>SUM A</t>
+  </si>
+  <si>
+    <t>_res_.$sum$B</t>
+  </si>
+  <si>
+    <t>_res_.$sum$C</t>
+  </si>
+  <si>
+    <t>_res_.$sum$E</t>
+  </si>
+  <si>
+    <t>_res_.$sum$F</t>
+  </si>
+  <si>
+    <t>_res_.$sum$H</t>
+  </si>
+  <si>
+    <t>9, 9</t>
+  </si>
+  <si>
+    <t>Test arrayCast</t>
+  </si>
+  <si>
+    <t>Test aliasCase4</t>
+  </si>
+  <si>
     <t>Spreadsheet MyAlias[] aliasCase4()</t>
   </si>
   <si>
-    <t>Test aliasCase4</t>
-  </si>
-  <si>
     <t>= new MyAlias[] {"One", "Other"}</t>
+  </si>
+  <si>
+    <t>, 6, 9, 6</t>
+  </si>
+  <si>
+    <t>2I : Integer[][]</t>
+  </si>
+  <si>
+    <t>2D : Double[][]</t>
+  </si>
+  <si>
+    <t>= $2I</t>
+  </si>
+  <si>
+    <t>6, 9, 6, ,</t>
+  </si>
+  <si>
+    <t>SUM B</t>
+  </si>
+  <si>
+    <t>SUM C</t>
+  </si>
+  <si>
+    <t>SUM D</t>
+  </si>
+  <si>
+    <t>SUM E</t>
+  </si>
+  <si>
+    <t>SUM F</t>
+  </si>
+  <si>
+    <t>SUM G</t>
+  </si>
+  <si>
+    <t>SUM H</t>
   </si>
 </sst>
 </file>
@@ -2287,7 +2377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2404,39 +2494,11 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2471,7 +2533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2517,12 +2579,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2532,10 +2595,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2859,10 +2922,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3086,28 +3149,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
@@ -4018,16 +4081,16 @@
       <c r="V28" s="4"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="24" t="s">
         <v>405</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
@@ -4642,28 +4705,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
@@ -5970,16 +6033,16 @@
       <c r="V28" s="4"/>
     </row>
     <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="24" t="s">
         <v>453</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="6" t="s">
@@ -6802,91 +6865,245 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:C19"/>
+  <dimension ref="B5:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="60.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
-        <v>684</v>
-      </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="C5" s="26"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>736</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>721</v>
+      </c>
+      <c r="H6" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
+        <v>712</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>673</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>723</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>724</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>705</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>725</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>740</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>714</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>726</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>741</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="C10" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="23" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
         <v>675</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>677</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>679</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>681</v>
-      </c>
       <c r="C11" s="17" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20">
-        <v>4</v>
+        <v>708</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>727</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>743</v>
+      </c>
+      <c r="J11" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>715</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>728</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="J12" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>710</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="23" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>717</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>711</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>729</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>746</v>
+      </c>
+      <c r="J14" t="s">
+        <v>730</v>
       </c>
     </row>
   </sheetData>
@@ -6902,8 +7119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6913,204 +7130,204 @@
     <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>687</v>
+        <v>678</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>688</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
+        <v>687</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="E11" s="27" t="s">
+        <v>688</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="H11" s="29" t="s">
+        <v>694</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="K11" s="27" t="s">
+        <v>733</v>
+      </c>
+      <c r="L11" s="28"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>692</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>692</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>704</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>692</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>693</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>699</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>700</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>686</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>698</v>
+      </c>
+      <c r="I19" s="29"/>
+      <c r="K19" s="19" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
+        <v>684</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>684</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>695</v>
+      </c>
+      <c r="I20" s="19" t="s">
         <v>696</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="E11" s="28" t="s">
+      <c r="K20" s="19" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="K21" s="19" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
+        <v>685</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>691</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>697</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="H11" s="30" t="s">
+      <c r="I22" s="19" t="s">
+        <v>678</v>
+      </c>
+      <c r="K22" s="19" t="s">
         <v>703</v>
-      </c>
-      <c r="I11" s="30"/>
-      <c r="K11" s="28" t="s">
-        <v>714</v>
-      </c>
-      <c r="L11" s="29"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>690</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>690</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>690</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>692</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>701</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>701</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>712</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>701</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>702</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>708</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>709</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="L14" s="22" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H15" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
-        <v>695</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>698</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>707</v>
-      </c>
-      <c r="I19" s="30"/>
-      <c r="K19" s="21" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
-        <v>693</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>693</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>705</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>365</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>365</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>365</v>
-      </c>
-      <c r="I21" s="21"/>
-      <c r="K21" s="21" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
-        <v>694</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>700</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>706</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>713</v>
-      </c>
-      <c r="K22" s="21" t="s">
-        <v>713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-8701 Issues with Date, Date[], DateRange constants in DTs
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastsTest.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71ED96E-54ED-465A-B2AD-4EDAF88EF558}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="11" r:id="rId1"/>
@@ -20,17 +21,24 @@
     <definedName name="_st2">#REF!</definedName>
     <definedName name="_st3">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="766">
   <si>
     <t>Step</t>
   </si>
@@ -2290,13 +2298,71 @@
   </si>
   <si>
     <t>SUM H</t>
+  </si>
+  <si>
+    <t>StringRange</t>
+  </si>
+  <si>
+    <t>= new StringRange('a');</t>
+  </si>
+  <si>
+    <t>= "Hello"</t>
+  </si>
+  <si>
+    <t>StringRange : StringRange</t>
+  </si>
+  <si>
+    <t>= (StringRange)$Types.$Value$String</t>
+  </si>
+  <si>
+    <t>= (StringRange)$Types.$Value$StringValue</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>= new Date();</t>
+  </si>
+  <si>
+    <t>DateRange</t>
+  </si>
+  <si>
+    <t>= new DateRange("1/1/2015 - 1/1/2017")</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>DateRange : DateRange</t>
+  </si>
+  <si>
+    <t>StringRage : StringRange</t>
+  </si>
+  <si>
+    <t>= (DateRange)$Types.$Value$Date</t>
+  </si>
+  <si>
+    <t>= (DateRange)$Types.$Value$LongValue</t>
+  </si>
+  <si>
+    <t>= (DateRange)$Types.$Value$Long</t>
+  </si>
+  <si>
+    <t>= $Types.$Value$Date</t>
+  </si>
+  <si>
+    <t>= (DateRange)((long) 0)</t>
+  </si>
+  <si>
+    <t>= new StringRange("a");</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2326,7 +2392,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.499984740745262" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -2338,6 +2404,12 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2348,19 +2420,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2372,7 +2444,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519241921" rgb="F79646"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2530,10 +2602,10 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2557,12 +2629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="6" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2606,8 +2672,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Accent1 10" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent1 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2623,9 +2689,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2663,9 +2729,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2698,9 +2764,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2733,9 +2816,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2908,24 +3008,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C5:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="65" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="65.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3105,12 +3205,36 @@
         <v>606</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="11" t="s">
+    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="4" t="s">
         <v>610</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>756</v>
       </c>
     </row>
   </sheetData>
@@ -3122,57 +3246,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:V62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C4:W65"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="18" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20" customWidth="1" collapsed="1"/>
-    <col min="20" max="22" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="15" max="18" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="20" max="22" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="24" t="s">
+    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-    </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+    </row>
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -3233,8 +3359,11 @@
       <c r="V5" s="5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W5" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -3295,88 +3424,94 @@
       <c r="V6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-    </row>
-    <row r="9" spans="3:22" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="3:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
@@ -3392,23 +3527,24 @@
       <c r="G10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-    </row>
-    <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
@@ -3427,22 +3563,23 @@
       <c r="H11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-    </row>
-    <row r="12" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
@@ -3464,21 +3601,22 @@
       <c r="I12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
@@ -3503,20 +3641,21 @@
       <c r="J13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-    </row>
-    <row r="14" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3535,24 +3674,25 @@
       <c r="H14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+    </row>
+    <row r="15" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
@@ -3583,78 +3723,81 @@
       <c r="L15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-    </row>
-    <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+    </row>
+    <row r="16" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-    </row>
-    <row r="17" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+    </row>
+    <row r="17" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="4" t="s">
         <v>50</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-    </row>
-    <row r="18" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
@@ -3670,11 +3813,11 @@
       <c r="G18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="4" t="s">
         <v>50</v>
       </c>
@@ -3684,15 +3827,16 @@
       <c r="O18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
@@ -3711,10 +3855,10 @@
       <c r="H19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="4" t="s">
         <v>50</v>
       </c>
@@ -3727,14 +3871,15 @@
       <c r="P19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-    </row>
-    <row r="20" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
@@ -3756,9 +3901,9 @@
       <c r="I20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
       <c r="M20" s="4" t="s">
         <v>50</v>
       </c>
@@ -3775,12 +3920,13 @@
         <v>54</v>
       </c>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-    </row>
-    <row r="21" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
@@ -3805,8 +3951,8 @@
       <c r="J21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="4" t="s">
         <v>50</v>
       </c>
@@ -3825,12 +3971,13 @@
       <c r="R21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-    </row>
-    <row r="22" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3849,12 +3996,12 @@
       <c r="H22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
       <c r="K22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="11"/>
       <c r="M22" s="4" t="s">
         <v>50</v>
       </c>
@@ -3867,16 +4014,17 @@
       <c r="P22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
       <c r="S22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-    </row>
-    <row r="23" spans="3:22" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="3:23" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
@@ -3931,260 +4079,282 @@
       <c r="T23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-    </row>
-    <row r="24" spans="3:22" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="3:23" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="4" t="s">
         <v>403</v>
       </c>
       <c r="V24" s="4" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="25" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
       <c r="V25" s="4" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="26" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>607</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="13"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-    </row>
-    <row r="27" spans="3:22" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>758</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="4" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="28" spans="3:23" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-    </row>
-    <row r="28" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="3" t="s">
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+    </row>
+    <row r="29" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="24" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I36" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="3" t="s">
+      <c r="K36" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4" t="s">
-        <v>407</v>
-      </c>
+      <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4" t="s">
-        <v>410</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>407</v>
-      </c>
+      <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>409</v>
-      </c>
+      <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>406</v>
@@ -4198,15 +4368,14 @@
       <c r="G40" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>408</v>
-      </c>
+      <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>406</v>
@@ -4223,14 +4392,13 @@
       <c r="H41" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I41" s="4" t="s">
-        <v>411</v>
-      </c>
+      <c r="I41" s="4"/>
       <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>406</v>
@@ -4250,13 +4418,12 @@
       <c r="I42" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="J42" s="4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>406</v>
@@ -4273,12 +4440,17 @@
       <c r="H43" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I43" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>406</v>
@@ -4295,66 +4467,72 @@
       <c r="H44" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>406</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>410</v>
-      </c>
+      <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>407</v>
-      </c>
+      <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>409</v>
-      </c>
+      <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>406</v>
@@ -4368,15 +4546,14 @@
       <c r="G48" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="H48" s="4" t="s">
-        <v>408</v>
-      </c>
+      <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>406</v>
@@ -4393,14 +4570,13 @@
       <c r="H49" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I49" s="4" t="s">
-        <v>411</v>
-      </c>
+      <c r="I49" s="4"/>
       <c r="J49" s="4"/>
-    </row>
-    <row r="50" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>406</v>
@@ -4420,13 +4596,12 @@
       <c r="I50" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="J50" s="4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="3:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>406</v>
@@ -4443,12 +4618,17 @@
       <c r="H51" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I51" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="3:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>406</v>
@@ -4465,34 +4645,40 @@
       <c r="H52" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I52" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="53" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="3:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
-        <v>607</v>
+        <v>41</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>407</v>
+      </c>
       <c r="F53" s="4" t="s">
         <v>410</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H53" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>406</v>
@@ -4507,228 +4693,290 @@
       <c r="H54" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="I54" s="4" t="s">
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55" spans="3:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="I55" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="J55" s="4" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="55" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4" t="s">
-        <v>612</v>
-      </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-    </row>
-    <row r="56" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="3:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>422</v>
-      </c>
+        <v>759</v>
+      </c>
+      <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
-    </row>
-    <row r="57" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K56" s="4" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="3" t="s">
-        <v>415</v>
+        <v>758</v>
       </c>
       <c r="D57" s="4"/>
-      <c r="E57" s="4" t="s">
-        <v>414</v>
-      </c>
+      <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>408</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
-    </row>
-    <row r="58" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="E58" s="13"/>
-      <c r="F58" s="4" t="s">
-        <v>435</v>
-      </c>
+        <v>611</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
-    </row>
-    <row r="59" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>436</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
-    </row>
-    <row r="60" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>421</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>440</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
-    </row>
-    <row r="61" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K60" s="4"/>
+    </row>
+    <row r="61" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+    </row>
+    <row r="62" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+    </row>
+    <row r="63" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+    </row>
+    <row r="64" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D64" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F64" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="G64" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="H64" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="I64" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="J61" s="4"/>
-    </row>
-    <row r="62" spans="3:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C62" s="3" t="s">
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+    </row>
+    <row r="65" spans="3:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E65" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F65" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G65" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="H65" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I65" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J65" s="4" t="s">
         <v>445</v>
       </c>
+      <c r="K65" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C4:V4"/>
-    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:K35"/>
+    <mergeCell ref="C4:W4"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:V60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="C4:W62"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="25" t="s">
+    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-    </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+    </row>
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -4789,8 +5037,11 @@
       <c r="V5" s="5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="6" spans="3:22" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W5" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -4851,8 +5102,11 @@
       <c r="V6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -4907,10 +5161,11 @@
       <c r="T7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
@@ -4965,10 +5220,11 @@
       <c r="T8" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-    </row>
-    <row r="9" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
@@ -5023,10 +5279,11 @@
       <c r="T9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
@@ -5081,10 +5338,11 @@
       <c r="T10" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-    </row>
-    <row r="11" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
@@ -5139,10 +5397,11 @@
       <c r="T11" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-    </row>
-    <row r="12" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
@@ -5197,10 +5456,11 @@
       <c r="T12" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
@@ -5255,10 +5515,11 @@
       <c r="T13" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-    </row>
-    <row r="14" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
@@ -5313,10 +5574,11 @@
       <c r="T14" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+    </row>
+    <row r="15" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
@@ -5371,10 +5633,11 @@
       <c r="T15" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-    </row>
-    <row r="16" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+    </row>
+    <row r="16" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
@@ -5429,10 +5692,11 @@
       <c r="T16" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-    </row>
-    <row r="17" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+    </row>
+    <row r="17" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
@@ -5487,10 +5751,11 @@
       <c r="T17" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-    </row>
-    <row r="18" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
@@ -5545,10 +5810,11 @@
       <c r="T18" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
@@ -5603,10 +5869,11 @@
       <c r="T19" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-    </row>
-    <row r="20" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
@@ -5661,10 +5928,11 @@
       <c r="T20" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-    </row>
-    <row r="21" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="3:23" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
@@ -5719,10 +5987,11 @@
       <c r="T21" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-    </row>
-    <row r="22" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="3:23" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
@@ -5777,10 +6046,11 @@
       <c r="T22" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-    </row>
-    <row r="23" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="3:23" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
@@ -5835,73 +6105,76 @@
       <c r="T23" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-    </row>
-    <row r="24" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="4" t="s">
         <v>394</v>
       </c>
       <c r="V24" s="4" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="25" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
       <c r="U25" s="4" t="s">
         <v>396</v>
       </c>
       <c r="V25" s="4" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="26" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>607</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="E26" s="13"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="4" t="s">
         <v>614</v>
       </c>
@@ -5947,17 +6220,18 @@
       <c r="T26" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-    </row>
-    <row r="27" spans="3:22" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="3:23" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>608</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="E27" s="13"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="4" t="s">
         <v>630</v>
       </c>
@@ -6003,770 +6277,846 @@
       <c r="T27" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-    </row>
-    <row r="28" spans="3:22" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+    </row>
+    <row r="28" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C32" s="24" t="s">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+    </row>
+    <row r="29" spans="3:23" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="30" spans="3:23" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="W30" s="4"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="22" t="s">
         <v>453</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I34" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>373</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="35" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>647</v>
+        <v>446</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="36" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
     </row>
     <row r="37" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>482</v>
+        <v>650</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="40" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="41" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="42" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="3" t="s">
+    <row r="43" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I43" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="43" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="3" t="s">
+    <row r="44" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I44" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J44" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="3" t="s">
+    <row r="45" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>513</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>655</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="46" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="48" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="49" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="50" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H51" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J51" s="4" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C51" s="3" t="s">
+    <row r="52" spans="3:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="4" t="s">
+      <c r="E52" s="11"/>
+      <c r="F52" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="H52" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I52" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="J51" s="4" t="s">
+      <c r="J52" s="4" t="s">
         <v>667</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>662</v>
-      </c>
-      <c r="E52" s="13"/>
-      <c r="F52" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>669</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>670</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>671</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="53" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
+        <v>608</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="54" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>557</v>
-      </c>
+        <v>758</v>
+      </c>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
       <c r="H54" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>764</v>
+      </c>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>561</v>
-      </c>
+        <v>611</v>
+      </c>
+      <c r="D55" s="11"/>
       <c r="E55" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>567</v>
-      </c>
+        <v>646</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
     </row>
     <row r="56" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="57" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>584</v>
+        <v>563</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>585</v>
+        <v>564</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>586</v>
+        <v>565</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>587</v>
+        <v>566</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>588</v>
+        <v>567</v>
       </c>
     </row>
     <row r="58" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="59" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="G61" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="I61" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="60" spans="3:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="3" t="s">
+    <row r="62" spans="3:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F62" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="G62" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="I62" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>602</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C4:V4"/>
-    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C4:W4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B8:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6775,7 +7125,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="51.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
@@ -6864,44 +7214,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B5:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="60.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>676</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>719</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>736</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>737</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>721</v>
       </c>
       <c r="H6" t="s">
@@ -6909,25 +7259,25 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>712</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>673</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="15" t="s">
         <v>720</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="16" t="s">
         <v>723</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="21" t="s">
         <v>724</v>
       </c>
       <c r="J7">
@@ -6935,25 +7285,25 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>713</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>705</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="15" t="s">
         <v>720</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="16" t="s">
         <v>725</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="21" t="s">
         <v>740</v>
       </c>
       <c r="J8">
@@ -6961,25 +7311,25 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>714</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>707</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>720</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="16" t="s">
         <v>726</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="21" t="s">
         <v>741</v>
       </c>
       <c r="J9">
@@ -6987,46 +7337,46 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>674</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>706</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>720</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="23" t="s">
+      <c r="H10" s="16"/>
+      <c r="I10" s="21" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>675</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>708</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>718</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="16" t="s">
         <v>727</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="21" t="s">
         <v>743</v>
       </c>
       <c r="J11" t="s">
@@ -7034,25 +7384,25 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>715</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>709</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="15" t="s">
         <v>718</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="16" t="s">
         <v>728</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="21" t="s">
         <v>744</v>
       </c>
       <c r="J12" t="s">
@@ -7060,46 +7410,46 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>716</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>710</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>718</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="23" t="s">
+      <c r="H13" s="16"/>
+      <c r="I13" s="21" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>717</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>711</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>718</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="16" t="s">
         <v>729</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="21" t="s">
         <v>746</v>
       </c>
       <c r="J14" t="s">
@@ -7116,7 +7466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B5:L22"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -7125,14 +7475,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -7161,172 +7511,172 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>687</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="E11" s="27" t="s">
+      <c r="C11" s="26"/>
+      <c r="E11" s="25" t="s">
         <v>688</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="H11" s="29" t="s">
+      <c r="F11" s="26"/>
+      <c r="H11" s="27" t="s">
         <v>694</v>
       </c>
-      <c r="I11" s="29"/>
-      <c r="K11" s="27" t="s">
+      <c r="I11" s="27"/>
+      <c r="K11" s="25" t="s">
         <v>733</v>
       </c>
-      <c r="L11" s="28"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>681</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="17" t="s">
         <v>681</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="17" t="s">
         <v>681</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="17" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>682</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>683</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>692</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="18" t="s">
         <v>690</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="17" t="s">
         <v>692</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="18" t="s">
         <v>704</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="17" t="s">
         <v>692</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="18" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>682</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="18" t="s">
         <v>693</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="17" t="s">
         <v>699</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="18" t="s">
         <v>700</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="17" t="s">
         <v>682</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="L14" s="18" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="17" t="s">
         <v>682</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="18" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>686</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="17" t="s">
         <v>689</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="27" t="s">
         <v>698</v>
       </c>
-      <c r="I19" s="29"/>
-      <c r="K19" s="19" t="s">
+      <c r="I19" s="27"/>
+      <c r="K19" s="17" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>684</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="17" t="s">
         <v>684</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="17" t="s">
         <v>695</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="17" t="s">
         <v>696</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="17" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>365</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="17" t="s">
         <v>365</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="17" t="s">
         <v>365</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="K21" s="19" t="s">
+      <c r="I21" s="17"/>
+      <c r="K21" s="17" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>685</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="17" t="s">
         <v>691</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="17" t="s">
         <v>697</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="17" t="s">
         <v>678</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="17" t="s">
         <v>703</v>
       </c>
     </row>

</xml_diff>